<commit_message>
Added mapping from EMPD country to Natural Earth country
</commit_message>
<xml_diff>
--- a/postgres/scripts/FixedTables.xlsx
+++ b/postgres/scripts/FixedTables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mchevali1/Research/EMPD2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/psommer/Documents/myplots-scripts/EMPD-data/postgres/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{384DC24C-5FD4-804E-BE7E-0304243970AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CFECA7-0C7C-4040-B084-B807BE5E7296}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26180" yWindow="8060" windowWidth="33320" windowHeight="23540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5080" yWindow="440" windowWidth="33320" windowHeight="21960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Country" sheetId="18" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="350">
   <si>
     <t>Country</t>
   </si>
@@ -1057,6 +1057,45 @@
   </si>
   <si>
     <t>archaeological</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Natural Earth</t>
   </si>
 </sst>
 </file>
@@ -1523,10 +1562,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:A86"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1661,434 +1700,683 @@
     <col min="16130" max="16130" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="4" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="40" spans="1:1">
+      <c r="B39" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="41" spans="1:1">
+      <c r="B40" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" s="4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="42" spans="1:1">
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:1">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="44" spans="1:1">
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="45" spans="1:1">
+      <c r="B44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="47" spans="1:1">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:1">
+      <c r="B47" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="B51" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:1">
+      <c r="B52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" s="4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="54" spans="1:1">
+      <c r="B53" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="55" spans="1:1">
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="56" spans="1:1">
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" s="4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" s="4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:1">
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="59" spans="1:1">
+      <c r="B58" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="60" spans="1:1">
+      <c r="B59" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="61" spans="1:1">
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="62" spans="1:1">
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="63" spans="1:1">
+      <c r="B62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" s="4" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="64" spans="1:1">
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
+      <c r="B64" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
+      <c r="B67" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" s="4" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
+      <c r="B68" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" s="4" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
+      <c r="B71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="74" spans="1:1">
+      <c r="B73" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="75" spans="1:1">
+      <c r="B74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="76" spans="1:1">
+      <c r="B75" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="77" spans="1:1">
+      <c r="B76" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="78" spans="1:1">
+      <c r="B77" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="79" spans="1:1">
+      <c r="B78" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="80" spans="1:1">
+      <c r="B79" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" s="14" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>334</v>
+      </c>
+      <c r="B86" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -2316,7 +2604,7 @@
   </sheetPr>
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>

</xml_diff>